<commit_message>
PSR-1505 - Content update - Asset from connected party data items updates
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Any asset other than land or property acquired from a connected party.xlsx
+++ b/conf/TEMPLATE - SIPP Any asset other than land or property acquired from a connected party.xlsx
@@ -149,13 +149,13 @@
     <t>Was the transaction supported by an independent valuation?</t>
   </si>
   <si>
+    <t>Has the asset been fully disposed of?</t>
+  </si>
+  <si>
     <t>Was there disposal of shares?</t>
   </si>
   <si>
     <t>If there were disposals of shares what is the total number of shares now held</t>
-  </si>
-  <si>
-    <t>If no disposals of shares were made has the asset been fully disposed of?</t>
   </si>
   <si>
     <r>
@@ -292,12 +292,13 @@
 Mandatory question if disposal of the asset was made.</t>
   </si>
   <si>
+    <t xml:space="preserve">Enter YES or NO.
+</t>
+  </si>
+  <si>
     <t>Min 1 - Max 7. 
-Use characters of 0-9.
-Mandatory question if disposal of the shares was made.</t>
-  </si>
-  <si>
-    <t>Enter YES or NO.
+0-9,999,999  Min 1 - Max 7 Characters of 0-9 
+If the asset has been fully disposed of and there was disposal of shares, then the number of shares now held must equal zero.
 Mandatory question if disposal of the shares was made.</t>
   </si>
 </sst>
@@ -367,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border/>
     <border>
       <right style="thin">
@@ -392,6 +393,20 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -400,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -430,6 +445,9 @@
     </xf>
     <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
@@ -750,7 +768,7 @@
       <c r="Y1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="10" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="8" t="s">
@@ -761,96 +779,96 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="11" t="s">
+      <c r="E2" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="15" t="s">
+      <c r="M2" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="15" t="s">
+      <c r="O2" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="13" t="s">
+      <c r="P2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="13" t="s">
+      <c r="Q2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="13" t="s">
+      <c r="R2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="13" t="s">
+      <c r="S2" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="13" t="s">
+      <c r="T2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="13" t="s">
+      <c r="U2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="13" t="s">
+      <c r="V2" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="13" t="s">
+      <c r="W2" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="13" t="s">
+      <c r="X2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="13" t="s">
+      <c r="Y2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="13" t="s">
+      <c r="Z2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA2" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="AA2" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB2" s="13" t="s">
+      <c r="AB2" s="14" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="3">
-      <c r="D3" s="16"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4">
-      <c r="D4" s="17"/>
+      <c r="D4" s="18"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
QuickFix - Excel fix
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Any asset other than land or property acquired from a connected party.xlsx
+++ b/conf/TEMPLATE - SIPP Any asset other than land or property acquired from a connected party.xlsx
@@ -1,12 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tolgahmrc/Projects/pension-scheme-return-sipp-frontend/conf/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA784EE-96C7-E141-8D37-27243B6F1F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Asset from a connected party" sheetId="1" r:id="rId4"/>
+    <sheet name="Asset from a connected party" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -15,19 +24,18 @@
   <si>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri, Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t>The questions in this section relate to any asset, other than land or property, acquired from a connected party.</t>
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri, Arial"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve"> 
 Questions that are mandatory are stated in row 2. Notes and hint text is underneath each question to help make sure that there are no errors in the template file upload.
@@ -36,39 +44,36 @@
     </r>
     <r>
       <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri, Arial"/>
-        <b/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">What you need to do
 </t>
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri, Arial"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t>Enter your data from row 3 onwards.</t>
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri, Arial"/>
-        <b val="0"/>
-        <color rgb="FFFF0000"/>
-        <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">
 </t>
     </r>
     <r>
       <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri, Arial"/>
-        <b val="0"/>
-        <color theme="1"/>
-        <sz val="12.0"/>
       </rPr>
       <t xml:space="preserve">
 Complete the questions per member marked horizontally across the columns. 
@@ -160,21 +165,20 @@
   <si>
     <r>
       <rPr>
-        <rFont val="Calibri, Arial"/>
         <b/>
         <i/>
+        <sz val="11"/>
         <color theme="1"/>
-        <sz val="11.0"/>
+        <rFont val="Calibri, Arial"/>
       </rPr>
       <t xml:space="preserve">Question help information. </t>
     </r>
     <r>
       <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
         <rFont val="Calibri, Arial"/>
-        <b val="0"/>
-        <i/>
-        <color theme="1"/>
-        <sz val="11.0"/>
       </rPr>
       <t>This will give you hints or tips to help you to complete the required cells.</t>
     </r>
@@ -224,17 +228,21 @@
   <si>
     <r>
       <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <color theme="1"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve">Max of 160 characters
 </t>
     </r>
     <r>
       <rPr>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
         <rFont val="Arial"/>
-        <i/>
-        <color theme="1"/>
+        <family val="2"/>
       </rPr>
       <t>Mandatory question if this was an acquisition of shares.</t>
     </r>
@@ -305,47 +313,84 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
-    <font>
-      <sz val="10.0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri, Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri, Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri, Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri, Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri, Arial"/>
     </font>
   </fonts>
   <fills count="4">
@@ -353,7 +398,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -369,16 +414,26 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -388,14 +443,18 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -410,83 +469,63 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -676,23 +715,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:AB2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD46"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="56.5"/>
+    <col min="1" max="1" width="56.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:28" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -714,31 +758,31 @@
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="5" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="7" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="5" t="s">
+      <c r="P1" s="4" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="3" t="s">
@@ -747,130 +791,124 @@
       <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="5" t="s">
+      <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="T1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="U1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="V1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="W1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="9" t="s">
+      <c r="X1" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="10" t="s">
+      <c r="Z1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="8" t="s">
+      <c r="AA1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="8" t="s">
+      <c r="AB1" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="11" t="s">
+    <row r="2" spans="1:28" ht="15.75" customHeight="1">
+      <c r="A2" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="14" t="s">
+      <c r="G2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="15" t="s">
+      <c r="K2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="M2" s="16" t="s">
+      <c r="M2" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="P2" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="Q2" s="14" t="s">
+      <c r="Q2" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="R2" s="14" t="s">
+      <c r="R2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="14" t="s">
+      <c r="S2" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="14" t="s">
+      <c r="T2" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="14" t="s">
+      <c r="V2" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="14" t="s">
+      <c r="W2" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="14" t="s">
+      <c r="X2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" s="14" t="s">
+      <c r="Y2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="Z2" s="14" t="s">
+      <c r="Z2" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="AA2" s="14" t="s">
+      <c r="AA2" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="8" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4">
-      <c r="D4" s="18"/>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[PSR-2048] Any asset other than land or property acquired from connected party template update
Update dependencies

Update sbt-plugin
</commit_message>
<xml_diff>
--- a/conf/TEMPLATE - SIPP Any asset other than land or property acquired from a connected party.xlsx
+++ b/conf/TEMPLATE - SIPP Any asset other than land or property acquired from a connected party.xlsx
@@ -9,7 +9,7 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="ha/+AWqU0NQwUwNRrNc/IojkEcWXc9LzAvAEdXTd7iI="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataChecksum="5VjDRhFXxoL8JjRHCt/JT6Z7zcIGeY9ts0FUbF0L8X4="/>
     </ext>
   </extLst>
 </workbook>
@@ -255,7 +255,7 @@
   </si>
   <si>
     <t xml:space="preserve">Enter the total amount in GBP (in pounds and pence).
-Enter amount as whole number and to two decimal places.
+Enter amount to two decimal places.
 If the asset was not an acquisition, provide the total market value.
 If the asset was acquired more than 6 years ago provide the market value at the year of the return
 Mandatory question
@@ -462,7 +462,7 @@
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="5" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="top" wrapText="1"/>

</xml_diff>